<commit_message>
fix for committed project import tests
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects_Good.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects_Good.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Source\Repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryson Taylor\Documents\Repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52064D44-2AA2-480D-8A41-C1AB0CFB185A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DBA955-A6B8-4C71-BD6C-27C5223B1C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8265" yWindow="14760" windowWidth="29700" windowHeight="19710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="4605" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Committed Projects" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>BMSID</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>+1</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>CapacityAdding</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,15 +473,15 @@
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -504,31 +510,34 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -556,8 +565,8 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2">
-        <v>1</v>
+      <c r="J2" t="s">
+        <v>25</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -568,8 +577,8 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
-        <v>18</v>
+      <c r="N2">
+        <v>1</v>
       </c>
       <c r="O2" t="s">
         <v>18</v>
@@ -580,8 +589,11 @@
       <c r="Q2" t="s">
         <v>18</v>
       </c>
+      <c r="R2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>3</v>
       </c>
@@ -606,10 +618,13 @@
       <c r="H3">
         <v>10000</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated test Excel file to include PROJECTSOURCE column
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects_Good.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/TestUtils/Files/TestCommittedProjects_Good.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryson Taylor\Documents\Repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swetherill\source\repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\TestUtils\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DBA955-A6B8-4C71-BD6C-27C5223B1C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB577B9-7D0A-4BDB-80B3-8293278DC1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="4605" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Committed Projects" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>BMSID</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>CapacityAdding</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>ProjectBuilder</t>
+  </si>
+  <si>
+    <t>PROJECTSOURCE</t>
   </si>
 </sst>
 </file>
@@ -457,31 +466,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -507,37 +518,40 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -563,14 +577,14 @@
         <v>250000</v>
       </c>
       <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
       <c r="L2">
         <v>1</v>
       </c>
@@ -580,8 +594,8 @@
       <c r="N2">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>18</v>
+      <c r="O2">
+        <v>1</v>
       </c>
       <c r="P2" t="s">
         <v>18</v>
@@ -592,8 +606,11 @@
       <c r="R2" t="s">
         <v>18</v>
       </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>3</v>
       </c>
@@ -618,13 +635,16 @@
       <c r="H3">
         <v>10000</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>